<commit_message>
fix(excel2json): write newlines correctly into the "description" field of the JSON file (RDU-45) (#1170)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/new_excel2json_files/json_header.xlsx
+++ b/testdata/excel2json/new_excel2json_files/json_header.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools-uv/testdata/excel2json/new_excel2json_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1587E9A-7A45-E14C-A520-49BA842A7F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374469-FE6E-6648-BE08-4EE49C65E73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="21880" windowWidth="25540" windowHeight="9000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,19 @@
     <sheet name="Keywords" sheetId="4" r:id="rId4"/>
     <sheet name="Users" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="eXIUItnczbsgwU2bhTxsCIaPyk1rdouaLJcS/mum0so="/>
     </ext>
@@ -302,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -312,6 +323,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6681,8 +6695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6734,14 +6748,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="4"/>
@@ -14837,7 +14851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+    <sheetView zoomScale="119" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>